<commit_message>
tutorial covid model revised
</commit_message>
<xml_diff>
--- a/tutorial/CovidContagion/data/input/id_age_group.xlsx
+++ b/tutorial/CovidContagion/data/input/id_age_group.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/ABM4ALL/Melodie/tutorial/CovidContagion/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F353AFC-DBAB-1441-A6F7-9487308A0F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64291F83-A90F-034C-8738-448915882C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2140" windowWidth="30240" windowHeight="12980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34360" yWindow="-2160" windowWidth="30240" windowHeight="12980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simulator_scenarios" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,14 +95,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -368,15 +378,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -410,10 +421,10 @@
         <v>0.8</v>
       </c>
       <c r="D2">
-        <v>0.19900000000000001</v>
+        <v>0.19899999999999995</v>
       </c>
       <c r="E2">
-        <v>1E-3</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -430,14 +441,17 @@
         <v>0.8</v>
       </c>
       <c r="D3">
-        <v>0.19</v>
+        <v>0.18999999999999995</v>
       </c>
       <c r="E3">
-        <v>0.01</v>
+        <v>1.0000000000000009E-2</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>